<commit_message>
update module 2 and files
</commit_message>
<xml_diff>
--- a/docs/officeAddress.xlsx
+++ b/docs/officeAddress.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>屏東</t>
   </si>
@@ -204,6 +204,18 @@
   </si>
   <si>
     <t>actgr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actgr_PCcarsNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actgr_CCcarsNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actgr_CCcarsRent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -257,11 +269,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,19 +559,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -569,8 +589,17 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -583,8 +612,17 @@
       <c r="D2" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>171000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -597,8 +635,17 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>173700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -611,8 +658,17 @@
       <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>175200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -625,8 +681,17 @@
       <c r="D5" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2">
+        <v>174480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -639,8 +704,17 @@
       <c r="D6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
+        <v>156401.32999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -653,8 +727,17 @@
       <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>175600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -667,8 +750,17 @@
       <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>159000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -681,8 +773,17 @@
       <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>170400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -695,8 +796,17 @@
       <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2">
+        <v>166950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -709,8 +819,17 @@
       <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>164100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -722,6 +841,15 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="2">
+        <v>171600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>